<commit_message>
fixed a wrong number in arrivalTime.csv
</commit_message>
<xml_diff>
--- a/CTA-railway/CTA-railway/simple_data/EXPLANATION.xlsx
+++ b/CTA-railway/CTA-railway/simple_data/EXPLANATION.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\CTA-optimal-control-under-incidents\simple_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\CTA-optimal-control-under-incidents\CTA-railway\CTA-railway\simple_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648B824D-22DF-4B52-928A-A9BA152FC905}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5E0484-B97A-4789-99D7-714DB4EA630F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11940" activeTab="1" xr2:uid="{1825468F-3913-41A2-9689-94FCDE51F798}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28776" windowHeight="11940" firstSheet="1" activeTab="5" xr2:uid="{1825468F-3913-41A2-9689-94FCDE51F798}"/>
   </bookViews>
   <sheets>
     <sheet name="stations" sheetId="4" r:id="rId1"/>
@@ -644,12 +644,12 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="10.875" customWidth="1"/>
+    <col min="3" max="4" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -666,7 +666,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -683,7 +683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -700,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -717,22 +717,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -747,13 +747,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9AF7CD-4EA7-4D92-81C9-C5F14D8EA680}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -767,7 +767,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -781,7 +781,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -795,7 +795,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -809,7 +809,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -823,7 +823,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -837,7 +837,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -851,7 +851,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -865,17 +865,17 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -895,9 +895,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -911,7 +911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -925,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -939,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -953,7 +953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -972,9 +972,9 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -985,7 +985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -996,7 +996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1070,9 +1070,9 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1149,22 +1149,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1180,16 +1180,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E2EAB8-4C91-42DA-A785-B9C6D472A7C6}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1216,10 +1216,10 @@
         <v>100</v>
       </c>
       <c r="C3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1242,10 +1242,10 @@
       </c>
       <c r="C5">
         <f>C3+300</f>
-        <v>360</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1268,10 +1268,10 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>660</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1294,10 +1294,10 @@
       </c>
       <c r="C9">
         <f t="shared" si="3"/>
-        <v>960</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1320,10 +1320,10 @@
       </c>
       <c r="C11">
         <f t="shared" si="5"/>
-        <v>1260</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1346,10 +1346,10 @@
       </c>
       <c r="C13">
         <f t="shared" si="7"/>
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1372,10 +1372,10 @@
       </c>
       <c r="C15">
         <f t="shared" si="9"/>
-        <v>1860</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>2260</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1398,10 +1398,10 @@
       </c>
       <c r="C17">
         <f t="shared" si="11"/>
-        <v>2160</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1424,10 +1424,10 @@
       </c>
       <c r="C19">
         <f t="shared" si="13"/>
-        <v>2460</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>2860</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1450,10 +1450,10 @@
       </c>
       <c r="C21">
         <f t="shared" si="15"/>
-        <v>2760</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2860</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>3160</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1476,10 +1476,10 @@
       </c>
       <c r="C23">
         <f t="shared" si="17"/>
-        <v>3060</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>3460</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1502,10 +1502,10 @@
       </c>
       <c r="C25">
         <f t="shared" si="19"/>
-        <v>3360</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3460</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>3760</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1528,20 +1528,20 @@
       </c>
       <c r="C27">
         <f t="shared" si="21"/>
-        <v>3660</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3760</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -1549,6 +1549,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1560,9 +1561,9 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1570,7 +1571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1581,7 +1582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1592,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1603,7 +1604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1614,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1625,7 +1626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1636,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1647,7 +1648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1658,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1669,7 +1670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1680,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1691,7 +1692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1702,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1713,7 +1714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1724,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1735,7 +1736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1746,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1757,7 +1758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1768,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1779,7 +1780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1790,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1801,7 +1802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1812,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1823,7 +1824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1834,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1856,17 +1857,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
@@ -1882,15 +1883,15 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F27"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.25" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1910,7 +1911,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1930,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1950,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1971,7 +1972,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1992,7 +1993,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -2013,7 +2014,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -2034,7 +2035,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -2076,7 +2077,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -2097,7 +2098,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -2118,7 +2119,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -2139,7 +2140,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -2160,7 +2161,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -2181,7 +2182,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -2202,7 +2203,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -2223,7 +2224,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -2244,7 +2245,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -2265,7 +2266,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -2286,7 +2287,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -2307,7 +2308,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -2328,7 +2329,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -2349,7 +2350,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2370,7 +2371,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2391,7 +2392,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -2412,7 +2413,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -2433,7 +2434,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -2454,7 +2455,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -2473,9 +2474,9 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2489,7 +2490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2517,7 +2518,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2531,12 +2532,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
functions can be called by python.
</commit_message>
<xml_diff>
--- a/CTA-railway/CTA-railway/simple_data/EXPLANATION.xlsx
+++ b/CTA-railway/CTA-railway/simple_data/EXPLANATION.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HuXiao\source\repos\CTA-optimal-control-under-incidents\CTA-railway\CTA-railway\simple_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0BECA2-BAC9-43CF-8786-82CFC8376B48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0376D7-F33C-45C0-BE90-A8ED58EAB1CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11940" xr2:uid="{1825468F-3913-41A2-9689-94FCDE51F798}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11940" activeTab="1" xr2:uid="{1825468F-3913-41A2-9689-94FCDE51F798}"/>
   </bookViews>
   <sheets>
     <sheet name="stations" sheetId="4" r:id="rId1"/>
-    <sheet name="fixOD" sheetId="10" r:id="rId2"/>
+    <sheet name="fixedOD" sheetId="10" r:id="rId2"/>
     <sheet name="policy_num" sheetId="1" r:id="rId3"/>
     <sheet name="policy" sheetId="2" r:id="rId4"/>
     <sheet name="direction" sheetId="3" r:id="rId5"/>
@@ -640,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4331848-2BA8-4AC2-929A-520C1CE3094F}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -747,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9AF7CD-4EA7-4D92-81C9-C5F14D8EA680}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
rebuild some functions, not yet finished
</commit_message>
<xml_diff>
--- a/CTA-railway/CTA-railway/simple_data/EXPLANATION.xlsx
+++ b/CTA-railway/CTA-railway/simple_data/EXPLANATION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HuXiao\source\repos\CTA-optimal-control-under-incidents\CTA-railway\CTA-railway\simple_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0376D7-F33C-45C0-BE90-A8ED58EAB1CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789876F5-686A-47A3-86CA-53268089B8DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11940" activeTab="1" xr2:uid="{1825468F-3913-41A2-9689-94FCDE51F798}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="fixedOD" sheetId="10" r:id="rId2"/>
     <sheet name="policy_num" sheetId="1" r:id="rId3"/>
     <sheet name="policy" sheetId="2" r:id="rId4"/>
-    <sheet name="direction" sheetId="3" r:id="rId5"/>
+    <sheet name="directions" sheetId="3" r:id="rId5"/>
     <sheet name="arrivalTime" sheetId="5" r:id="rId6"/>
     <sheet name="arrivalStationID" sheetId="6" r:id="rId7"/>
     <sheet name="startTrainInfo" sheetId="7" r:id="rId8"/>

</xml_diff>